<commit_message>
E2E testcasese for Febreze.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Febreze/FebrezeTestData.xlsx
+++ b/src/test/resources/TestData/Febreze/FebrezeTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\New folder (3)\HoT-digital1 (1)\HoT-digital1\src\test\resources\TestData\Febreze\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkJEE!\stinger and Febreze code\HoT-digital\src\test\resources\TestData\Febreze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB76CB48-D852-4E52-B8E4-0DF369345DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4007C6BE-C859-486A-B4B4-82307364A260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C5FE9447-98AF-4C4C-A51B-4FE645A2C407}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="99">
   <si>
     <t>DataSet</t>
   </si>
@@ -132,18 +132,9 @@
     <t>AccountDetails</t>
   </si>
   <si>
-    <t>divyasreesrivastava@gmail.com</t>
-  </si>
-  <si>
-    <t>DivyaSree@123</t>
-  </si>
-  <si>
     <t>AccountCreation</t>
   </si>
   <si>
-    <t>rajkumar@gmaill.com</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -303,9 +294,6 @@
     <t>Febreze</t>
   </si>
   <si>
-    <t>saikatipelli@gmail.com</t>
-  </si>
-  <si>
     <t>Air Purifier</t>
   </si>
   <si>
@@ -328,6 +316,12 @@
   </si>
   <si>
     <t>MasterCard</t>
+  </si>
+  <si>
+    <t>rpotharaju@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>123123@Qa</t>
   </si>
 </sst>
 </file>
@@ -337,7 +331,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +372,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -406,7 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
@@ -425,6 +425,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -742,18 +743,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE0F8F46-FA12-4FB8-B45F-D560233EE084}">
   <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" customWidth="1"/>
     <col min="7" max="7" width="33.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
@@ -807,7 +808,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>13</v>
@@ -825,7 +826,7 @@
         <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>18</v>
@@ -881,75 +882,75 @@
         <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>35</v>
+        <v>88</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" t="s">
         <v>40</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>41</v>
-      </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" t="s">
-        <v>44</v>
       </c>
       <c r="L4">
         <v>72018</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="R4">
         <v>9.375</v>
@@ -957,26 +958,26 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="P5" s="6">
         <v>2021</v>
       </c>
       <c r="Q5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="R5" s="4">
         <v>737</v>
@@ -984,17 +985,17 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O6" s="5">
         <v>1212121212121210</v>
@@ -1003,7 +1004,7 @@
         <v>2021</v>
       </c>
       <c r="Q6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="R6" s="4">
         <v>737</v>
@@ -1011,152 +1012,152 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" t="s">
         <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" t="s">
-        <v>52</v>
-      </c>
-      <c r="K7" t="s">
-        <v>53</v>
       </c>
       <c r="L7" s="7">
         <v>12345</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F8" s="2"/>
       <c r="L8" s="7"/>
       <c r="M8" s="4"/>
       <c r="S8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="S9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="S10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" t="s">
         <v>59</v>
       </c>
-      <c r="D12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" t="s">
-        <v>62</v>
-      </c>
       <c r="K12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L12">
         <v>12345</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="O12" s="7"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="P13">
         <v>2023</v>
       </c>
       <c r="Q13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="R13">
         <v>731</v>
@@ -1164,25 +1165,25 @@
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
+        <v>88</v>
+      </c>
+      <c r="N14" t="s">
         <v>91</v>
       </c>
-      <c r="N14" t="s">
-        <v>95</v>
-      </c>
       <c r="O14" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P14">
         <v>2023</v>
       </c>
       <c r="Q14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="R14">
         <v>731</v>
@@ -1190,25 +1191,25 @@
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="P15">
         <v>2023</v>
       </c>
       <c r="Q15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="R15">
         <v>7314</v>
@@ -1216,126 +1217,126 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" t="s">
         <v>69</v>
       </c>
-      <c r="D16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" t="s">
-        <v>75</v>
-      </c>
-      <c r="I16" t="s">
-        <v>71</v>
-      </c>
-      <c r="J16" t="s">
-        <v>72</v>
-      </c>
       <c r="K16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L16">
         <v>23456</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" t="s">
         <v>73</v>
       </c>
-      <c r="D17" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="J17" t="s">
         <v>74</v>
       </c>
-      <c r="H17" t="s">
+      <c r="K17" t="s">
         <v>75</v>
-      </c>
-      <c r="I17" t="s">
-        <v>76</v>
-      </c>
-      <c r="J17" t="s">
-        <v>77</v>
-      </c>
-      <c r="K17" t="s">
-        <v>78</v>
       </c>
       <c r="L17">
         <v>98987</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20" t="s">
+        <v>87</v>
+      </c>
+      <c r="J20" t="s">
         <v>81</v>
       </c>
-      <c r="B20" t="s">
+      <c r="K20" t="s">
         <v>82</v>
-      </c>
-      <c r="D20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I20" t="s">
-        <v>90</v>
-      </c>
-      <c r="J20" t="s">
-        <v>84</v>
-      </c>
-      <c r="K20" t="s">
-        <v>85</v>
       </c>
       <c r="L20">
         <v>86380</v>
@@ -1346,28 +1347,19 @@
     </row>
     <row r="21" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="T21" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{59F3BD19-FD89-440C-8EB1-821B7B4F8C27}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{C7B34E85-1B98-407F-B9ED-DF86477054A6}"/>
-    <hyperlink ref="F12" r:id="rId3" display="harish.chiruvella1@gmail.com" xr:uid="{8DC793C4-05FF-4129-B1FF-EC22D124D8B9}"/>
-    <hyperlink ref="F16" r:id="rId4" display="harish.chiruvella1@gmail.com" xr:uid="{959671EE-24C4-4FE3-AD6B-19D50F097382}"/>
-    <hyperlink ref="F17" r:id="rId5" display="harish.chiruvella1@gmail.com" xr:uid="{EC36E94C-E228-4538-BDB2-883DA902F1C5}"/>
-    <hyperlink ref="C2" r:id="rId6" xr:uid="{F9B4D864-3A01-4E9E-BB9D-B5725BCFD66D}"/>
-    <hyperlink ref="F2" r:id="rId7" display="rajkumarpotharaju97@gmail.com" xr:uid="{F5F2BBD1-8B98-4E9C-B369-321F249AA3CC}"/>
-    <hyperlink ref="C3" r:id="rId8" xr:uid="{B5F89277-A4A6-4F2C-9403-E4FFD85BA6C1}"/>
-    <hyperlink ref="F3" r:id="rId9" xr:uid="{75F764FD-59A0-4BFC-A1FC-6FB5ABBAF8D3}"/>
-    <hyperlink ref="F20" r:id="rId10" display="harish.chiruvella1@gmail.com" xr:uid="{39D87703-A4F2-489D-BFE1-7F3EAE0524E4}"/>
-    <hyperlink ref="F4" r:id="rId11" xr:uid="{D97D9B9A-CF69-48DA-A2F6-24BD8E1D38FA}"/>
-    <hyperlink ref="F7" r:id="rId12" xr:uid="{00B7D06B-12C8-4CFA-888A-A3449BC440C4}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{F9B4D864-3A01-4E9E-BB9D-B5725BCFD66D}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{F925E518-9EA2-4D7D-8E07-6C29677D96AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>